<commit_message>
Committing changes to excels and charts
</commit_message>
<xml_diff>
--- a/categorical_indicators_summary.xlsx
+++ b/categorical_indicators_summary.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://msfintl-my.sharepoint.com/personal/krystel_moussally_msf_org/Documents/OneDrive Updated/7_MENA branch/MEMU/WHO_EWI/AMR_ProxyInd/Analysis/R-project/scoping_amr_indicators/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="11_ABE05A5B8614669AD6C54952F37BD272FA4FF49E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A19622EE-80FB-4CB9-8871-0DF187F8EEB0}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="11_ABE05A5B8614669AD6C54952F37BD272FA4FF49E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B428555-AC19-4B6D-B9F3-6DEF67CAB6D9}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary_cat_indicators" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">summary_cat_indicators!$A$1:$E$55</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
@@ -792,10 +795,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="38.54296875" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
@@ -825,7 +829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="5" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="5" customFormat="1" ht="409.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -842,7 +846,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="5" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="5" customFormat="1" ht="409.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -859,7 +863,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="5" customFormat="1" ht="143" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="5" customFormat="1" ht="143" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -876,7 +880,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="5" customFormat="1" ht="65" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="5" customFormat="1" ht="65" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
@@ -893,7 +897,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="5" customFormat="1" ht="65" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" s="5" customFormat="1" ht="65" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
@@ -910,7 +914,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="5" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="5" customFormat="1" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>2</v>
       </c>
@@ -927,7 +931,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="7" customFormat="1" ht="130" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" s="7" customFormat="1" ht="130" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>15</v>
       </c>
@@ -944,7 +948,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="5" customFormat="1" ht="143" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="5" customFormat="1" ht="143" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>18</v>
       </c>
@@ -961,7 +965,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="5" customFormat="1" ht="65" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" s="5" customFormat="1" ht="65" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
@@ -978,7 +982,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="5" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" s="5" customFormat="1" ht="39" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -995,7 +999,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="7" customFormat="1" ht="234" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" s="7" customFormat="1" ht="234" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>25</v>
       </c>
@@ -1012,7 +1016,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="7" customFormat="1" ht="260" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" s="7" customFormat="1" ht="260" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>25</v>
       </c>
@@ -1029,7 +1033,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="7" customFormat="1" ht="273" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" s="7" customFormat="1" ht="286" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>25</v>
       </c>
@@ -1046,7 +1050,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="7" customFormat="1" ht="117" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" s="7" customFormat="1" ht="117" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
         <v>25</v>
       </c>
@@ -1063,7 +1067,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="7" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" s="7" customFormat="1" ht="39" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>25</v>
       </c>
@@ -1080,7 +1084,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>25</v>
       </c>
@@ -1097,7 +1101,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="7" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" s="7" customFormat="1" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
         <v>25</v>
       </c>
@@ -1114,7 +1118,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="5" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" s="5" customFormat="1" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>40</v>
       </c>
@@ -1131,7 +1135,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="5" customFormat="1" ht="52" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" s="5" customFormat="1" ht="65" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>40</v>
       </c>
@@ -1148,7 +1152,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="5" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" s="5" customFormat="1" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>40</v>
       </c>
@@ -1165,7 +1169,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="5" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" s="5" customFormat="1" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>40</v>
       </c>
@@ -1182,7 +1186,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>40</v>
       </c>
@@ -1199,7 +1203,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="7" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" s="7" customFormat="1" ht="409.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
         <v>51</v>
       </c>
@@ -1216,7 +1220,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="7" customFormat="1" ht="247" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" s="7" customFormat="1" ht="260" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
         <v>51</v>
       </c>
@@ -1233,7 +1237,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="7" customFormat="1" ht="117" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" s="7" customFormat="1" ht="117" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
         <v>51</v>
       </c>
@@ -1250,7 +1254,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="7" customFormat="1" ht="130" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" s="7" customFormat="1" ht="130" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
         <v>51</v>
       </c>
@@ -1267,7 +1271,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="7" customFormat="1" ht="91" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" s="7" customFormat="1" ht="91" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
         <v>51</v>
       </c>
@@ -1284,7 +1288,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="7" customFormat="1" ht="65" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" s="7" customFormat="1" ht="65" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="8" t="s">
         <v>51</v>
       </c>
@@ -1301,7 +1305,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="5" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" s="5" customFormat="1" ht="409.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="6" t="s">
         <v>64</v>
       </c>
@@ -1318,7 +1322,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="5" customFormat="1" ht="234" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" s="5" customFormat="1" ht="247" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
         <v>64</v>
       </c>
@@ -1335,7 +1339,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="5" customFormat="1" ht="182" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" s="5" customFormat="1" ht="195" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
         <v>64</v>
       </c>
@@ -1352,7 +1356,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="5" customFormat="1" ht="299" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" s="5" customFormat="1" ht="312" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
         <v>64</v>
       </c>
@@ -1369,7 +1373,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="5" customFormat="1" ht="104" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" s="5" customFormat="1" ht="104" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
         <v>64</v>
       </c>
@@ -1386,7 +1390,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="5" customFormat="1" ht="117" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" s="5" customFormat="1" ht="117" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
         <v>64</v>
       </c>
@@ -1403,7 +1407,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="5" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" s="5" customFormat="1" ht="27.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
         <v>64</v>
       </c>
@@ -1420,7 +1424,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="5" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" s="5" customFormat="1" ht="27.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
         <v>64</v>
       </c>
@@ -1437,7 +1441,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="7" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" s="7" customFormat="1" ht="409.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="8" t="s">
         <v>81</v>
       </c>
@@ -1454,7 +1458,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="7" customFormat="1" ht="195" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" s="7" customFormat="1" ht="208" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="8" t="s">
         <v>81</v>
       </c>
@@ -1471,7 +1475,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="7" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" s="7" customFormat="1" ht="39" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="8" t="s">
         <v>81</v>
       </c>
@@ -1488,7 +1492,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="5" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" s="5" customFormat="1" ht="409.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="6" t="s">
         <v>88</v>
       </c>
@@ -1505,7 +1509,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="7" customFormat="1" ht="195" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" s="7" customFormat="1" ht="208" x14ac:dyDescent="0.35">
       <c r="A42" s="8" t="s">
         <v>90</v>
       </c>
@@ -1590,7 +1594,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="5" customFormat="1" ht="169" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" s="5" customFormat="1" ht="169" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6" t="s">
         <v>101</v>
       </c>
@@ -1607,7 +1611,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="5" customFormat="1" ht="117" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" s="5" customFormat="1" ht="117" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="6" t="s">
         <v>101</v>
       </c>
@@ -1624,7 +1628,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="5" customFormat="1" ht="104" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" s="5" customFormat="1" ht="104" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
         <v>101</v>
       </c>
@@ -1641,7 +1645,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="5" customFormat="1" ht="78" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" s="5" customFormat="1" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="6" t="s">
         <v>101</v>
       </c>
@@ -1658,7 +1662,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="5" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" s="5" customFormat="1" ht="39" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="6" t="s">
         <v>101</v>
       </c>
@@ -1675,7 +1679,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="5" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" s="5" customFormat="1" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="6" t="s">
         <v>101</v>
       </c>
@@ -1692,7 +1696,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" s="5" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
         <v>101</v>
       </c>
@@ -1709,7 +1713,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="5" customFormat="1" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" s="5" customFormat="1" ht="21.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="6" t="s">
         <v>101</v>
       </c>
@@ -1726,7 +1730,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="7" customFormat="1" ht="169" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" s="7" customFormat="1" ht="182" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="8" t="s">
         <v>118</v>
       </c>
@@ -1744,6 +1748,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E55" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Patient outcomes"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>